<commit_message>
Updated OL Documentation(Excel) for the comments.
</commit_message>
<xml_diff>
--- a/testing/OamLog+testcase.docs.xlsx
+++ b/testing/OamLog+testcase.docs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venka\Documents\MW\OL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31461770-2FE5-4C08-9B67-F6C448BC8216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5137041-03DF-4F47-A6D6-85FC39E47E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{8A4BF7CC-909B-4C1B-B59F-29AF2D960B3A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="226">
   <si>
     <t>Testcases</t>
   </si>
@@ -1183,24 +1183,6 @@
 </t>
   </si>
   <si>
-    <t>#### Requires:
-- ExecutionAndTraceLog server to operate
-- ApplicationLayerTopology server to operate</t>
-  </si>
-  <si>
-    <t>#### Testing:
-- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP, protocol and port from above
-   - operation-key from above
-   - DummyValue of x-correlator
-   - checking response 
-   - checking same record for containing DummyXCorrelator and application-name=applicationName from list retrieved from /v1/list-end-points-of-link, operation-name=update-operation-ket, trace-indicator=expected unique trace-indicator(values appened with unique numbers) and other attributes as expected.</t>
-  </si>
-  <si>
-    <t>"#### Clearing:
-- not applicable"</t>
-  </si>
-  <si>
     <t>#### Testing:
 - POST ExecutionAndTraceLog/v1/list-records-of-flow with 
    - IP, protocol and port from above
@@ -1238,26 +1220,6 @@
 each callback is present .
 POST - 3 min - eatl log -x-core - check entries
 timer 10 min - loop for every 1 min, to check if last forwarding is executed/not</t>
-  </si>
-  <si>
-    <t>#### Preparation:
-- GETing CC (/core-model-1-4:control-construct)
-  - search CC for output fc-port of ServiceRequestCausesLoggingRequest, 
-its corresponding op-c, http-c and tcp-c, storing them for later verification request
-  - searching CC for output-fc-port of ServiceRequestCausesLtpUpdateRequest, its corresponding op-c, http-c, storing them.
-  - searching CC for output-fc-port of CyclicOperationCausesRequestForListOfLinks, its corresponding op-c, storing them.
-  - searching CC for output-fc-port of CyclicOperationCausesRequestForLinkEndPoints, its corresponding op-c, storing them.
-   - searching CC for op-s of /v1/regard-updated-link storing operation-key
-- GETting EaTL/CC (while using IP, protocol and port from above)
-   - searching CC for op-c of /v1/list-records-of-flow, storing operation-key
-- POST ALT/v1/list-link-uuids - For getting link-uuid
-  - randonly select a link-uuid and store it
-- POST ALT/v1/list-end-points-of-link - For getting link end points
- - extract Link End Point list from response-body and store it 
-- POST /v1/regard-updated-link with  
-   - attribute according to randomly chosen link-uuid from above
-   -operation-key from above
-   - all parameters with realistic values (incl. DummyXCorrelator)</t>
   </si>
   <si>
     <t>#### Testing:
@@ -1409,6 +1371,16 @@
 - checking for ResponseCode==204
 - POST /v1/list-records-of-application and store response
 - verify that received response is equal to expected attribute values ( ex: application-name = ExpectedApplicationName, release-number = expectedReleaseNumber, method= expectedMethod, resource = expectedResource, etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#### Testing:
+- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
+   - IP, protocol and port from above
+   - operation-key from above
+   - DummyValue of x-correlator
+   - checking response 
+   - checking same record for containing DummyXCorrelator and applicatin-name and release-number with randomly chosen values.
+</t>
   </si>
 </sst>
 </file>
@@ -1877,6 +1849,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1886,7 +1859,6 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -2206,10 +2178,10 @@
   <dimension ref="A1:I223"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B117" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2269,17 +2241,17 @@
         <v>88</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="63" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -2315,7 +2287,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="62"/>
+      <c r="A5" s="63"/>
       <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
@@ -2415,7 +2387,7 @@
 &amp;CONCATENATE("
 - POST ",I3,"
     - operation-key from above
-    - all attributes filled with random value
+    - attribute according to chosen http-c
     - reasonable parameters")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
@@ -2423,12 +2395,12 @@
   - searching CC for output fc-port of NewApplicationCausesRequestForOamRequestInformation, find corresponding http-c, store them
 - POST /v1/list-records-of-application
     - operation-key from above
-    - all attributes filled with random value
+    - attribute according to chosen http-c
     - reasonable parameters</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="62"/>
+      <c r="A6" s="63"/>
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
@@ -2473,7 +2445,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A7" s="62"/>
+      <c r="A7" s="63"/>
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
@@ -2512,7 +2484,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="62" t="s">
+      <c r="A8" s="63" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -2548,7 +2520,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="62"/>
+      <c r="A9" s="63"/>
       <c r="B9" s="8" t="s">
         <v>10</v>
       </c>
@@ -2647,6 +2619,7 @@
 &amp;CONCATENATE("
   - POST ",I3,"
     - operation-key from above
+    - attribute according to chosen http-c
     - BUT one randomly chosen parameter (user, originator, x-correlator, trace-indicator or customer-journey) missing (not empty string!)")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
@@ -2654,11 +2627,12 @@
   - searching CC for output fc-port of NewApplicationCausesRequestForOamRequestInformation, find corresponding http-c, store them
   - POST /v1/list-records-of-application
     - operation-key from above
+    - attribute according to chosen http-c
     - BUT one randomly chosen parameter (user, originator, x-correlator, trace-indicator or customer-journey) missing (not empty string!)</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="62"/>
+      <c r="A10" s="63"/>
       <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
@@ -2699,7 +2673,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A11" s="62"/>
+      <c r="A11" s="63"/>
       <c r="B11" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -2740,7 +2714,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="62" t="s">
+      <c r="A12" s="63" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -2776,7 +2750,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="203" x14ac:dyDescent="0.35">
-      <c r="A13" s="62"/>
+      <c r="A13" s="63"/>
       <c r="B13" s="8" t="s">
         <v>14</v>
       </c>
@@ -2875,19 +2849,21 @@
   - searching CC for output fc-port of NewApplicationCausesRequestForOamRequestInformation, find corresponding http-c, store them")
 &amp;CONCATENATE("
   - POST ",I$3,"
-      - all parameters with realistic values, BUT 
+       - attribute according to chosen http-c
+       - all parameters with realistic values, BUT 
           1.  originator set to be a string of 0, 1 or 2 (random) letters length (too short).")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
   - searching CC for op-s of /v1/list-records-of-application, storing operation-key
   - searching CC for output fc-port of NewApplicationCausesRequestForOamRequestInformation, find corresponding http-c, store them
   - POST /v1/list-records-of-application
-      - all parameters with realistic values, BUT 
+       - attribute according to chosen http-c
+       - all parameters with realistic values, BUT 
           1.  originator set to be a string of 0, 1 or 2 (random) letters length (too short).</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="62"/>
+      <c r="A14" s="63"/>
       <c r="B14" s="8" t="s">
         <v>15</v>
       </c>
@@ -2928,7 +2904,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A15" s="62"/>
+      <c r="A15" s="63"/>
       <c r="B15" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -2969,7 +2945,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="62" t="s">
+      <c r="A16" s="63" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -3005,7 +2981,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="203" x14ac:dyDescent="0.35">
-      <c r="A17" s="62"/>
+      <c r="A17" s="63"/>
       <c r="B17" s="8" t="s">
         <v>18</v>
       </c>
@@ -3104,7 +3080,7 @@
 &amp;CONCATENATE("
   - POST ",I$3,"
     - operation-key from above
-    - all attributes filled with random value
+    - attribute according to chosen http-c
     - reasonable parameters, BUT dummyXCorrelators differing from the pattern in various ways (e.g. empty string)")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
@@ -3112,12 +3088,12 @@
   - searching CC for output fc-port of NewApplicationCausesRequestForOamRequestInformation, find corresponding http-c, store them
   - POST /v1/list-records-of-application
     - operation-key from above
-    - all attributes filled with random value
+    - attribute according to chosen http-c
     - reasonable parameters, BUT dummyXCorrelators differing from the pattern in various ways (e.g. empty string)</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="62"/>
+      <c r="A18" s="63"/>
       <c r="B18" s="8" t="s">
         <v>15</v>
       </c>
@@ -3158,7 +3134,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A19" s="62"/>
+      <c r="A19" s="63"/>
       <c r="B19" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -3199,7 +3175,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="62" t="s">
+      <c r="A20" s="63" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -3235,7 +3211,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="203" x14ac:dyDescent="0.35">
-      <c r="A21" s="62"/>
+      <c r="A21" s="63"/>
       <c r="B21" s="8" t="s">
         <v>21</v>
       </c>
@@ -3334,7 +3310,7 @@
 &amp;CONCATENATE("
   - POST ",I$3,"
     - operation-key from above
-    - all attributes filled with random value
+    - attribute according to chosen http-c
     - reasonable parameters, BUT dummyTraceIndicator differing from the pattern in various ways (e.g. empty string)")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
@@ -3342,12 +3318,12 @@
   - searching CC for output fc-port of NewApplicationCausesRequestForOamRequestInformation, find corresponding http-c, store them
   - POST /v1/list-records-of-application
     - operation-key from above
-    - all attributes filled with random value
+    - attribute according to chosen http-c
     - reasonable parameters, BUT dummyTraceIndicator differing from the pattern in various ways (e.g. empty string)</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="62"/>
+      <c r="A22" s="63"/>
       <c r="B22" s="8" t="s">
         <v>15</v>
       </c>
@@ -3388,7 +3364,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A23" s="62"/>
+      <c r="A23" s="63"/>
       <c r="B23" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -3429,7 +3405,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="62" t="s">
+      <c r="A24" s="63" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -3465,7 +3441,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="62"/>
+      <c r="A25" s="63"/>
       <c r="B25" s="8" t="s">
         <v>24</v>
       </c>
@@ -3543,18 +3519,20 @@
   - searching CC for output fc-port of NewApplicationCausesRequestForOamRequestInformation, find corresponding http-c, store them")
 &amp;CONCATENATE("
 - POST ",I$3,"
+    - attribute according to chosen http-c
     - reasonable parameters
     - BUT operationKey parameter missing (does not mean empty string)")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
   - searching CC for output fc-port of NewApplicationCausesRequestForOamRequestInformation, find corresponding http-c, store them
 - POST /v1/list-records-of-application
+    - attribute according to chosen http-c
     - reasonable parameters
     - BUT operationKey parameter missing (does not mean empty string)</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="62"/>
+      <c r="A26" s="63"/>
       <c r="B26" s="8" t="s">
         <v>25</v>
       </c>
@@ -3595,7 +3573,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="62"/>
+      <c r="A27" s="63"/>
       <c r="B27" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -3636,7 +3614,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="62" t="s">
+      <c r="A28" s="63" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="7" t="s">
@@ -3672,7 +3650,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="62"/>
+      <c r="A29" s="63"/>
       <c r="B29" s="8" t="s">
         <v>28</v>
       </c>
@@ -3750,18 +3728,20 @@
   - searching CC for output fc-port of NewApplicationCausesRequestForOamRequestInformation, find corresponding http-c, store them")
 &amp;CONCATENATE("
 - POST ",I$3,"
-    - reasonable parameters
+     - attribute according to chosen http-c
+     - reasonable parameters
      - BUT operationKey parameter with random dummy value")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
   - searching CC for output fc-port of NewApplicationCausesRequestForOamRequestInformation, find corresponding http-c, store them
 - POST /v1/list-records-of-application
-    - reasonable parameters
+     - attribute according to chosen http-c
+     - reasonable parameters
      - BUT operationKey parameter with random dummy value</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="62"/>
+      <c r="A30" s="63"/>
       <c r="B30" s="8" t="s">
         <v>25</v>
       </c>
@@ -3802,7 +3782,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A31" s="62"/>
+      <c r="A31" s="63"/>
       <c r="B31" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -3843,7 +3823,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="62" t="s">
+      <c r="A32" s="63" t="s">
         <v>29</v>
       </c>
       <c r="B32" s="7" t="s">
@@ -3879,7 +3859,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="62"/>
+      <c r="A33" s="63"/>
       <c r="B33" s="8" t="s">
         <v>31</v>
       </c>
@@ -3952,12 +3932,12 @@
   - searching CC for output fc-port of NewApplicationCausesRequestForOamRequestInformation, find corresponding http-c, store them
 - POST /v1/list-records-of-application
     - operation-key from above
-    - all attributes filled with random value
+    - attribute according to chosen http-c
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A34" s="62"/>
+    <row r="34" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="63"/>
       <c r="B34" s="8" t="s">
         <v>32</v>
       </c>
@@ -3982,17 +3962,15 @@
       <c r="G34" s="48" t="s">
         <v>119</v>
       </c>
-      <c r="H34" s="29">
-        <f>$J34</f>
-        <v>0</v>
-      </c>
-      <c r="I34" s="29">
-        <f>$J34</f>
-        <v>0</v>
+      <c r="H34" s="48" t="s">
+        <v>119</v>
+      </c>
+      <c r="I34" s="48" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A35" s="62"/>
+      <c r="A35" s="63"/>
       <c r="B35" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -4033,7 +4011,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" s="62" t="s">
+      <c r="A36" s="63" t="s">
         <v>33</v>
       </c>
       <c r="B36" s="7" t="s">
@@ -4069,7 +4047,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="62"/>
+      <c r="A37" s="63"/>
       <c r="B37" s="8" t="s">
         <v>31</v>
       </c>
@@ -4142,12 +4120,12 @@
   - searching CC for output fc-port of NewApplicationCausesRequestForOamRequestInformation, find corresponding http-c, store them
 - POST /v1/list-records-of-application
     - operation-key from above
-    - all attributes filled with random value
+    - attribute according to chosen http-c
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="62"/>
+    <row r="38" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A38" s="63"/>
       <c r="B38" s="8" t="s">
         <v>35</v>
       </c>
@@ -4175,17 +4153,15 @@
       <c r="G38" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="H38" s="25">
-        <f>$J38</f>
-        <v>0</v>
-      </c>
-      <c r="I38" s="25">
-        <f>$J38</f>
-        <v>0</v>
+      <c r="H38" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="I38" s="48" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A39" s="62"/>
+      <c r="A39" s="63"/>
       <c r="B39" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -4226,7 +4202,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" s="62" t="s">
+      <c r="A40" s="63" t="s">
         <v>36</v>
       </c>
       <c r="B40" s="7" t="s">
@@ -4262,7 +4238,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="63"/>
+      <c r="A41" s="64"/>
       <c r="B41" s="8" t="s">
         <v>31</v>
       </c>
@@ -4335,12 +4311,12 @@
   - searching CC for output fc-port of NewApplicationCausesRequestForOamRequestInformation, find corresponding http-c, store them
 - POST /v1/list-records-of-application
     - operation-key from above
-    - all attributes filled with random value
+    - attribute according to chosen http-c
     - reasonable parameters</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="63"/>
+      <c r="A42" s="64"/>
       <c r="B42" s="8" t="s">
         <v>38</v>
       </c>
@@ -4402,7 +4378,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A43" s="63"/>
+      <c r="A43" s="64"/>
       <c r="B43" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -4443,7 +4419,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="62" t="s">
+      <c r="A44" s="63" t="s">
         <v>39</v>
       </c>
       <c r="B44" s="7" t="s">
@@ -4472,7 +4448,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="63"/>
+      <c r="A45" s="64"/>
       <c r="B45" s="8" t="s">
         <v>41</v>
       </c>
@@ -4499,7 +4475,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="246.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="63"/>
+      <c r="A46" s="64"/>
       <c r="B46" s="8" t="s">
         <v>185</v>
       </c>
@@ -4651,7 +4627,7 @@
    - searching CC for op-c of /v1/list-records-of-flow, storing operation-key
 - POST ",I3,"-
   - operation-key from above
-  - all attributes filled with random values
+  - attribute according to chosen http-c
   - reasonable parameters")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
@@ -4663,17 +4639,17 @@
    - searching CC for op-c of /v1/list-records-of-flow, storing operation-key
 - POST /v1/list-records-of-application-
   - operation-key from above
-  - all attributes filled with random values
+  - attribute according to chosen http-c
   - reasonable parameters</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="63"/>
+      <c r="A47" s="64"/>
       <c r="B47" s="8" t="s">
         <v>186</v>
       </c>
       <c r="C47" s="29" t="str">
-        <f>CONCATENATE("#### Testing:
+        <f t="shared" ref="C47:I47" si="29">CONCATENATE("#### Testing:
 - POST ExecutionAndTraceLog/v1/list-records-of-flow with 
    - IP, protocol and port from above
    - operation-key from above
@@ -4689,13 +4665,7 @@
    - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator</v>
       </c>
       <c r="D47" s="29" t="str">
-        <f>CONCATENATE("#### Testing:
-- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP, protocol and port from above
-   - operation-key from above
-   - DummyValue of x-correlator
-   - checking response for entry with application-name==OamLog and operation-name==", D3, "
-   - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator")</f>
+        <f t="shared" si="29"/>
         <v>#### Testing:
 - POST ExecutionAndTraceLog/v1/list-records-of-flow with 
    - IP, protocol and port from above
@@ -4705,13 +4675,7 @@
    - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator</v>
       </c>
       <c r="E47" s="29" t="str">
-        <f>CONCATENATE("#### Testing:
-- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP, protocol and port from above
-   - operation-key from above
-   - DummyValue of x-correlator
-   - checking response for entry with application-name==OamLog and operation-name==", E3, "
-   - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator")</f>
+        <f t="shared" si="29"/>
         <v>#### Testing:
 - POST ExecutionAndTraceLog/v1/list-records-of-flow with 
    - IP, protocol and port from above
@@ -4721,13 +4685,7 @@
    - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator</v>
       </c>
       <c r="F47" s="29" t="str">
-        <f>CONCATENATE("#### Testing:
-- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP, protocol and port from above
-   - operation-key from above
-   - DummyValue of x-correlator
-   - checking response for entry with application-name==OamLog and operation-name==", F3, "
-   - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator")</f>
+        <f t="shared" si="29"/>
         <v>#### Testing:
 - POST ExecutionAndTraceLog/v1/list-records-of-flow with 
    - IP, protocol and port from above
@@ -4737,13 +4695,7 @@
    - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator</v>
       </c>
       <c r="G47" s="29" t="str">
-        <f>CONCATENATE("#### Testing:
-- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP, protocol and port from above
-   - operation-key from above
-   - DummyValue of x-correlator
-   - checking response for entry with application-name==OamLog and operation-name==", G3, "
-   - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator")</f>
+        <f t="shared" si="29"/>
         <v>#### Testing:
 - POST ExecutionAndTraceLog/v1/list-records-of-flow with 
    - IP, protocol and port from above
@@ -4753,13 +4705,7 @@
    - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator</v>
       </c>
       <c r="H47" s="29" t="str">
-        <f>CONCATENATE("#### Testing:
-- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP, protocol and port from above
-   - operation-key from above
-   - DummyValue of x-correlator
-   - checking response for entry with application-name==OamLog and operation-name==", H3, "
-   - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator")</f>
+        <f t="shared" si="29"/>
         <v>#### Testing:
 - POST ExecutionAndTraceLog/v1/list-records-of-flow with 
    - IP, protocol and port from above
@@ -4769,13 +4715,7 @@
    - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator</v>
       </c>
       <c r="I47" s="29" t="str">
-        <f>CONCATENATE("#### Testing:
-- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP, protocol and port from above
-   - operation-key from above
-   - DummyValue of x-correlator
-   - checking response for entry with application-name==OamLog and operation-name==", I3, "
-   - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator")</f>
+        <f t="shared" si="29"/>
         <v>#### Testing:
 - POST ExecutionAndTraceLog/v1/list-records-of-flow with 
    - IP, protocol and port from above
@@ -4786,7 +4726,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="63"/>
+      <c r="A48" s="64"/>
       <c r="B48" s="9" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -4796,32 +4736,32 @@
         <v>124</v>
       </c>
       <c r="D48" s="32" t="str">
-        <f>$B7</f>
+        <f t="shared" ref="D48:I48" si="30">$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="E48" s="32" t="str">
-        <f>$B7</f>
+        <f t="shared" si="30"/>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="F48" s="32" t="str">
-        <f>$B7</f>
+        <f t="shared" si="30"/>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="G48" s="32" t="str">
-        <f>$B7</f>
+        <f t="shared" si="30"/>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="H48" s="32" t="str">
-        <f>$B7</f>
+        <f t="shared" si="30"/>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="I48" s="32" t="str">
-        <f>$B7</f>
+        <f t="shared" si="30"/>
         <v>#### Clearing:
 - not applicable</v>
       </c>
@@ -4837,10 +4777,10 @@
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
-      <c r="I49" s="65"/>
+      <c r="I49" s="62"/>
     </row>
     <row r="50" spans="1:9" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="64" t="s">
+      <c r="A50" s="65" t="s">
         <v>43</v>
       </c>
       <c r="B50" s="11" t="s">
@@ -4869,7 +4809,7 @@
       </c>
     </row>
     <row r="51" spans="1:9" ht="153.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="62"/>
+      <c r="A51" s="63"/>
       <c r="B51" s="12" t="s">
         <v>45</v>
       </c>
@@ -4920,7 +4860,7 @@
   - searching CC for output fc-port of NewApplicationCausesRequestForOamRequestInformation, find corresponding http-c, store them
 - POST ",I3," with
      - operation-key from above
-     - all attributes filled with random value
+     - attribute according to chosen http-c
       - reasonable parameters ")</f>
         <v xml:space="preserve">#### Preparation:
 - GETing CC (/core-model-1-4:control-construct
@@ -4928,12 +4868,12 @@
   - searching CC for output fc-port of NewApplicationCausesRequestForOamRequestInformation, find corresponding http-c, store them
 - POST /v1/list-records-of-application with
      - operation-key from above
-     - all attributes filled with random value
+     - attribute according to chosen http-c
       - reasonable parameters </v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="171" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="62"/>
+      <c r="A52" s="63"/>
       <c r="B52" s="13" t="s">
         <v>46</v>
       </c>
@@ -4947,7 +4887,7 @@
         <v>90</v>
       </c>
       <c r="F52" s="51" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G52" s="51"/>
       <c r="H52" s="24" t="s">
@@ -4958,7 +4898,7 @@
       </c>
     </row>
     <row r="53" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A53" s="62"/>
+      <c r="A53" s="63"/>
       <c r="B53" s="14" t="s">
         <v>47</v>
       </c>
@@ -4989,7 +4929,7 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A54" s="63" t="s">
+      <c r="A54" s="64" t="s">
         <v>48</v>
       </c>
       <c r="B54" s="11" t="s">
@@ -5012,7 +4952,7 @@
       </c>
     </row>
     <row r="55" spans="1:9" ht="174" x14ac:dyDescent="0.35">
-      <c r="A55" s="63"/>
+      <c r="A55" s="64"/>
       <c r="B55" s="12" t="s">
         <v>50</v>
       </c>
@@ -5054,7 +4994,7 @@
       </c>
     </row>
     <row r="56" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A56" s="63"/>
+      <c r="A56" s="64"/>
       <c r="B56" s="13" t="s">
         <v>51</v>
       </c>
@@ -5075,7 +5015,7 @@
       </c>
     </row>
     <row r="57" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="63"/>
+      <c r="A57" s="64"/>
       <c r="B57" s="14" t="s">
         <v>47</v>
       </c>
@@ -5096,7 +5036,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A58" s="63"/>
+      <c r="A58" s="64"/>
       <c r="B58" s="13" t="s">
         <v>52</v>
       </c>
@@ -5115,7 +5055,7 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A59" s="62" t="s">
+      <c r="A59" s="63" t="s">
         <v>53</v>
       </c>
       <c r="B59" s="7" t="s">
@@ -5138,20 +5078,20 @@
         <v>## Gets lifeCycleState propagated?</v>
       </c>
       <c r="G59" s="20" t="str">
-        <f t="shared" ref="G59:I59" si="29">$B$59</f>
+        <f t="shared" ref="G59:I59" si="31">$B$59</f>
         <v>## Gets lifeCycleState propagated?</v>
       </c>
       <c r="H59" s="20" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>## Gets lifeCycleState propagated?</v>
       </c>
       <c r="I59" s="20" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>## Gets lifeCycleState propagated?</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="203" x14ac:dyDescent="0.35">
-      <c r="A60" s="63"/>
+      <c r="A60" s="64"/>
       <c r="B60" s="8" t="s">
         <v>55</v>
       </c>
@@ -5259,8 +5199,8 @@
 - PUTting op-s-configuration/life-cycle-state with random alternative value")
 &amp;CONCATENATE("
 - POST ",I3,"
-    -operation-key from above
-    - all attributes filled with random value
+    - operation-key from above
+    - attribute according to chosen http-c
     - reasonable parameters")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
@@ -5268,13 +5208,13 @@
   - searching CC for output fc-port of NewApplicationCausesRequestForOamRequestInformation, find corresponding http-c, store them
 - PUTting op-s-configuration/life-cycle-state with random alternative value
 - POST /v1/list-records-of-application
-    -operation-key from above
-    - all attributes filled with random value
+    - operation-key from above
+    - attribute according to chosen http-c
     - reasonable parameters</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A61" s="63"/>
+      <c r="A61" s="64"/>
       <c r="B61" s="8" t="s">
         <v>56</v>
       </c>
@@ -5301,7 +5241,7 @@
       </c>
     </row>
     <row r="62" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="63"/>
+      <c r="A62" s="64"/>
       <c r="B62" s="15" t="s">
         <v>57</v>
       </c>
@@ -5328,7 +5268,7 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A63" s="62" t="s">
+      <c r="A63" s="63" t="s">
         <v>58</v>
       </c>
       <c r="B63" s="7" t="s">
@@ -5351,12 +5291,12 @@
         <v>## Get attributes checked for completeness?</v>
       </c>
       <c r="G63" s="20" t="str">
-        <f t="shared" ref="G63" si="30">$B$63</f>
+        <f t="shared" ref="G63" si="32">$B$63</f>
         <v>## Get attributes checked for completeness?</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="203" x14ac:dyDescent="0.35">
-      <c r="A64" s="62"/>
+      <c r="A64" s="63"/>
       <c r="B64" s="8" t="s">
         <v>60</v>
       </c>
@@ -5421,7 +5361,7 @@
       </c>
     </row>
     <row r="65" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A65" s="62"/>
+      <c r="A65" s="63"/>
       <c r="B65" s="8" t="s">
         <v>61</v>
       </c>
@@ -5450,7 +5390,7 @@
       </c>
     </row>
     <row r="66" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="62"/>
+      <c r="A66" s="63"/>
       <c r="B66" s="15" t="s">
         <v>47</v>
       </c>
@@ -5479,7 +5419,7 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A67" s="62" t="s">
+      <c r="A67" s="63" t="s">
         <v>133</v>
       </c>
       <c r="B67" s="7" t="s">
@@ -5502,12 +5442,12 @@
         <v>## Get each attributes checked for correctness?</v>
       </c>
       <c r="G67" s="20" t="str">
-        <f t="shared" ref="G67" si="31">$B$67</f>
+        <f t="shared" ref="G67" si="33">$B$67</f>
         <v>## Get each attributes checked for correctness?</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A68" s="62"/>
+      <c r="A68" s="63"/>
       <c r="B68" s="8"/>
       <c r="C68" s="41" t="s">
         <v>94</v>
@@ -5526,7 +5466,7 @@
       </c>
     </row>
     <row r="69" spans="1:7" ht="203" x14ac:dyDescent="0.35">
-      <c r="A69" s="62"/>
+      <c r="A69" s="63"/>
       <c r="B69" s="8"/>
       <c r="C69" s="21" t="s">
         <v>169</v>
@@ -5579,7 +5519,7 @@
       </c>
     </row>
     <row r="70" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="62"/>
+      <c r="A70" s="63"/>
       <c r="B70" s="8"/>
       <c r="C70" s="25" t="str">
         <f ca="1">$C70</f>
@@ -5599,7 +5539,7 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A71" s="62"/>
+      <c r="A71" s="63"/>
       <c r="B71" s="8"/>
       <c r="C71" s="22" t="str">
         <f>$B15</f>
@@ -5623,7 +5563,7 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A72" s="62"/>
+      <c r="A72" s="63"/>
       <c r="B72" s="8"/>
       <c r="C72" s="41" t="s">
         <v>157</v>
@@ -5636,7 +5576,7 @@
       </c>
     </row>
     <row r="73" spans="1:7" ht="203" x14ac:dyDescent="0.35">
-      <c r="A73" s="62"/>
+      <c r="A73" s="63"/>
       <c r="B73" s="8"/>
       <c r="C73" s="21" t="s">
         <v>170</v>
@@ -5679,7 +5619,7 @@
       </c>
     </row>
     <row r="74" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A74" s="62"/>
+      <c r="A74" s="63"/>
       <c r="B74" s="8"/>
       <c r="C74" s="25" t="str">
         <f ca="1">$C74</f>
@@ -5698,10 +5638,10 @@
       </c>
     </row>
     <row r="75" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A75" s="62"/>
+      <c r="A75" s="63"/>
       <c r="B75" s="8"/>
       <c r="C75" s="50" t="str">
-        <f t="shared" ref="C75" si="32">$B35</f>
+        <f t="shared" ref="C75" si="34">$B35</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
@@ -5717,7 +5657,7 @@
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A76" s="62"/>
+      <c r="A76" s="63"/>
       <c r="B76" s="8"/>
       <c r="C76" s="41" t="s">
         <v>95</v>
@@ -5726,11 +5666,11 @@
         <v>165</v>
       </c>
       <c r="G76" s="41" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="203" x14ac:dyDescent="0.35">
-      <c r="A77" s="62"/>
+      <c r="A77" s="63"/>
       <c r="B77" s="8"/>
       <c r="C77" s="21" t="s">
         <v>147</v>
@@ -5773,7 +5713,7 @@
       </c>
     </row>
     <row r="78" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A78" s="62"/>
+      <c r="A78" s="63"/>
       <c r="B78" s="8"/>
       <c r="C78" s="25" t="str">
         <f ca="1">$C78</f>
@@ -5792,7 +5732,7 @@
       </c>
     </row>
     <row r="79" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A79" s="62"/>
+      <c r="A79" s="63"/>
       <c r="B79" s="8"/>
       <c r="C79" s="22" t="str">
         <f>$B15</f>
@@ -5800,7 +5740,7 @@
 - not applicable</v>
       </c>
       <c r="D79" s="50" t="str">
-        <f t="shared" ref="D79" si="33">$B35</f>
+        <f t="shared" ref="D79" si="35">$B35</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
@@ -5811,7 +5751,7 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A80" s="62"/>
+      <c r="A80" s="63"/>
       <c r="B80" s="8"/>
       <c r="C80" s="41" t="s">
         <v>96</v>
@@ -5820,11 +5760,11 @@
         <v>135</v>
       </c>
       <c r="G80" s="41" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="203" x14ac:dyDescent="0.35">
-      <c r="A81" s="62"/>
+      <c r="A81" s="63"/>
       <c r="B81" s="8"/>
       <c r="C81" s="21" t="s">
         <v>148</v>
@@ -5867,7 +5807,7 @@
       </c>
     </row>
     <row r="82" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A82" s="62"/>
+      <c r="A82" s="63"/>
       <c r="B82" s="8"/>
       <c r="C82" s="25" t="str">
         <f ca="1">$C82</f>
@@ -5886,7 +5826,7 @@
       </c>
     </row>
     <row r="83" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83" s="62"/>
+      <c r="A83" s="63"/>
       <c r="B83" s="8"/>
       <c r="C83" s="22" t="str">
         <f>$B19</f>
@@ -5905,7 +5845,7 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A84" s="62"/>
+      <c r="A84" s="63"/>
       <c r="B84" s="8"/>
       <c r="C84" s="22"/>
       <c r="D84" s="41" t="s">
@@ -5913,7 +5853,7 @@
       </c>
     </row>
     <row r="85" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A85" s="62"/>
+      <c r="A85" s="63"/>
       <c r="B85" s="8"/>
       <c r="C85" s="22"/>
       <c r="D85" s="21" t="str">
@@ -5937,7 +5877,7 @@
       </c>
     </row>
     <row r="86" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A86" s="62"/>
+      <c r="A86" s="63"/>
       <c r="B86" s="8"/>
       <c r="C86" s="22"/>
       <c r="D86" s="25" t="str">
@@ -5948,7 +5888,7 @@
       <c r="G86" s="21"/>
     </row>
     <row r="87" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A87" s="62"/>
+      <c r="A87" s="63"/>
       <c r="B87" s="8"/>
       <c r="C87" s="22"/>
       <c r="D87" s="22" t="str">
@@ -5959,7 +5899,7 @@
       <c r="G87" s="25"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A88" s="62" t="s">
+      <c r="A88" s="63" t="s">
         <v>63</v>
       </c>
       <c r="B88" s="7" t="s">
@@ -5987,7 +5927,7 @@
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A89" s="62"/>
+      <c r="A89" s="63"/>
       <c r="B89" s="8"/>
       <c r="C89" s="41" t="s">
         <v>155</v>
@@ -6002,11 +5942,11 @@
         <v>90</v>
       </c>
       <c r="G89" s="41" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="303" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="63"/>
+      <c r="A90" s="64"/>
       <c r="B90" s="8" t="s">
         <v>65</v>
       </c>
@@ -6023,11 +5963,11 @@
         <v>90</v>
       </c>
       <c r="G90" s="21" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="105.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="63"/>
+      <c r="A91" s="64"/>
       <c r="B91" s="8" t="s">
         <v>66</v>
       </c>
@@ -6044,11 +5984,11 @@
         <v>90</v>
       </c>
       <c r="G91" s="25" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A92" s="63"/>
+      <c r="A92" s="64"/>
       <c r="B92" s="8" t="s">
         <v>47</v>
       </c>
@@ -6083,11 +6023,11 @@
         <v>102</v>
       </c>
       <c r="G93" s="24" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A94" s="62"/>
+      <c r="A94" s="63"/>
       <c r="B94" s="8"/>
       <c r="C94" s="41" t="s">
         <v>97</v>
@@ -6104,7 +6044,7 @@
       <c r="G94" s="41"/>
     </row>
     <row r="95" spans="1:7" ht="250.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="63"/>
+      <c r="A95" s="64"/>
       <c r="B95" s="8" t="s">
         <v>65</v>
       </c>
@@ -6112,7 +6052,7 @@
         <v>159</v>
       </c>
       <c r="D95" s="21" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E95" s="21"/>
       <c r="F95" s="52" t="s">
@@ -6123,7 +6063,7 @@
       </c>
     </row>
     <row r="96" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A96" s="63"/>
+      <c r="A96" s="64"/>
       <c r="B96" s="8" t="s">
         <v>66</v>
       </c>
@@ -6140,7 +6080,7 @@
       <c r="G96" s="25"/>
     </row>
     <row r="97" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A97" s="63"/>
+      <c r="A97" s="64"/>
       <c r="B97" s="8" t="s">
         <v>47</v>
       </c>
@@ -6187,7 +6127,7 @@
         <v>163</v>
       </c>
       <c r="D100" s="21" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
@@ -6237,7 +6177,7 @@
         <v>162</v>
       </c>
       <c r="D105" s="21" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
@@ -6306,7 +6246,7 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A114" s="62" t="s">
+      <c r="A114" s="63" t="s">
         <v>67</v>
       </c>
       <c r="B114" s="7" t="s">
@@ -6329,7 +6269,7 @@
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A115" s="62"/>
+      <c r="A115" s="63"/>
       <c r="B115" s="12"/>
       <c r="C115" s="42" t="s">
         <v>109</v>
@@ -6342,11 +6282,11 @@
         <v>90</v>
       </c>
       <c r="G115" s="59" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A116" s="63"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A116" s="64"/>
       <c r="B116" s="8" t="s">
         <v>69</v>
       </c>
@@ -6367,11 +6307,11 @@
         <v>90</v>
       </c>
       <c r="G116" s="24" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" ht="319" x14ac:dyDescent="0.35">
-      <c r="A117" s="63"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="275.5" x14ac:dyDescent="0.35">
+      <c r="A117" s="64"/>
       <c r="B117" s="8" t="s">
         <v>193</v>
       </c>
@@ -6379,7 +6319,7 @@
         <v>194</v>
       </c>
       <c r="D117" s="44" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E117" s="43" t="s">
         <v>90</v>
@@ -6388,19 +6328,19 @@
         <v>90</v>
       </c>
       <c r="G117" s="60" t="s">
-        <v>208</v>
+        <v>90</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A118" s="63"/>
+      <c r="A118" s="64"/>
       <c r="B118" s="8" t="s">
         <v>187</v>
       </c>
       <c r="C118" s="31" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D118" s="31" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E118" s="43" t="s">
         <v>90</v>
@@ -6409,11 +6349,11 @@
         <v>90</v>
       </c>
       <c r="G118" s="51" t="s">
-        <v>202</v>
+        <v>90</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A119" s="63"/>
+      <c r="A119" s="64"/>
       <c r="B119" s="5" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -6424,7 +6364,11 @@
         <v>#### Clearing:
 - not applicable</v>
       </c>
-      <c r="D119" s="45"/>
+      <c r="D119" s="45" t="str">
+        <f>$B7</f>
+        <v>#### Clearing:
+- not applicable</v>
+      </c>
       <c r="E119" s="43" t="s">
         <v>90</v>
       </c>
@@ -6432,11 +6376,11 @@
         <v>90</v>
       </c>
       <c r="G119" s="61" t="s">
-        <v>203</v>
+        <v>90</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A120" s="62" t="s">
+      <c r="A120" s="63" t="s">
         <v>70</v>
       </c>
       <c r="B120" s="11" t="s">
@@ -6459,13 +6403,13 @@
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A121" s="62"/>
+      <c r="A121" s="63"/>
       <c r="B121" s="13"/>
       <c r="C121" s="39" t="s">
         <v>90</v>
       </c>
       <c r="D121" s="39" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E121" s="39" t="s">
         <v>110</v>
@@ -6473,9 +6417,12 @@
       <c r="F121" s="39" t="s">
         <v>90</v>
       </c>
+      <c r="G121" s="52" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="122" spans="1:7" ht="237.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="62"/>
+      <c r="A122" s="63"/>
       <c r="B122" s="12" t="s">
         <v>72</v>
       </c>
@@ -6491,9 +6438,12 @@
       <c r="F122" s="39" t="s">
         <v>90</v>
       </c>
+      <c r="G122" s="52" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="123" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A123" s="62"/>
+      <c r="A123" s="63"/>
       <c r="B123" s="13" t="s">
         <v>73</v>
       </c>
@@ -6501,17 +6451,20 @@
         <v>90</v>
       </c>
       <c r="D123" s="25" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E123" s="24" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F123" s="39" t="s">
         <v>90</v>
       </c>
+      <c r="G123" s="52" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="124" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A124" s="62"/>
+      <c r="A124" s="63"/>
       <c r="B124" s="13" t="s">
         <v>47</v>
       </c>
@@ -6524,7 +6477,7 @@
       </c>
     </row>
     <row r="125" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A125" s="62"/>
+      <c r="A125" s="63"/>
       <c r="B125" s="13" t="s">
         <v>52</v>
       </c>
@@ -6537,7 +6490,7 @@
       </c>
     </row>
     <row r="126" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A126" s="62" t="s">
+      <c r="A126" s="63" t="s">
         <v>74</v>
       </c>
       <c r="B126" s="7" t="s">
@@ -6560,7 +6513,7 @@
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A127" s="62"/>
+      <c r="A127" s="63"/>
       <c r="B127" s="8"/>
       <c r="C127" s="41" t="s">
         <v>152</v>
@@ -6574,9 +6527,12 @@
       <c r="F127" s="39" t="s">
         <v>90</v>
       </c>
+      <c r="G127" s="52" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="128" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A128" s="62"/>
+      <c r="A128" s="63"/>
       <c r="B128" s="8" t="s">
         <v>41</v>
       </c>
@@ -6592,9 +6548,12 @@
       <c r="F128" s="39" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" ht="388.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="62"/>
+      <c r="G128" s="52" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="388.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A129" s="63"/>
       <c r="B129" s="8" t="s">
         <v>188</v>
       </c>
@@ -6610,21 +6569,24 @@
       <c r="F129" s="39" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" ht="145" x14ac:dyDescent="0.35">
-      <c r="A130" s="62"/>
+      <c r="G129" s="52" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+      <c r="A130" s="63"/>
       <c r="B130" s="8" t="s">
         <v>190</v>
       </c>
       <c r="C130" s="29" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D130" s="29" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A131" s="62"/>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A131" s="63"/>
       <c r="B131" s="8" t="s">
         <v>47</v>
       </c>
@@ -6635,8 +6597,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A132" s="62"/>
+    <row r="132" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A132" s="63"/>
       <c r="B132" s="13" t="s">
         <v>52</v>
       </c>
@@ -6647,8 +6609,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A133" s="62"/>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A133" s="63"/>
       <c r="B133" s="8"/>
       <c r="C133" s="41" t="s">
         <v>112</v>
@@ -6663,8 +6625,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A134" s="62"/>
+    <row r="134" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A134" s="63"/>
       <c r="B134" s="8" t="s">
         <v>41</v>
       </c>
@@ -6681,8 +6643,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="290" x14ac:dyDescent="0.35">
-      <c r="A135" s="62"/>
+    <row r="135" spans="1:7" ht="290" x14ac:dyDescent="0.35">
+      <c r="A135" s="63"/>
       <c r="B135" s="8" t="s">
         <v>188</v>
       </c>
@@ -6690,7 +6652,7 @@
         <v>191</v>
       </c>
       <c r="D135" s="21" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E135" s="39" t="s">
         <v>90</v>
@@ -6699,20 +6661,20 @@
         <v>90</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="145" x14ac:dyDescent="0.35">
-      <c r="A136" s="62"/>
+    <row r="136" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+      <c r="A136" s="63"/>
       <c r="B136" s="8" t="s">
         <v>190</v>
       </c>
       <c r="C136" s="29" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D136" s="29" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A137" s="62"/>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A137" s="63"/>
       <c r="B137" s="8" t="s">
         <v>47</v>
       </c>
@@ -6723,8 +6685,8 @@
         <v>167</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A138" s="62"/>
+    <row r="138" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A138" s="63"/>
       <c r="B138" s="13" t="s">
         <v>52</v>
       </c>
@@ -6735,8 +6697,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A139" s="62"/>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A139" s="63"/>
       <c r="B139" s="8"/>
       <c r="C139" s="41" t="s">
         <v>151</v>
@@ -6748,8 +6710,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A140" s="62"/>
+    <row r="140" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A140" s="63"/>
       <c r="B140" s="8"/>
       <c r="C140" s="31" t="s">
         <v>41</v>
@@ -6758,28 +6720,28 @@
         <v>41</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="62"/>
+    <row r="141" spans="1:7" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A141" s="63"/>
       <c r="B141" s="8"/>
       <c r="C141" s="21" t="s">
         <v>192</v>
       </c>
       <c r="D141" s="21" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A142" s="62"/>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A142" s="63"/>
       <c r="B142" s="8"/>
       <c r="C142" s="29" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D142" s="29" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A143" s="62"/>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A143" s="63"/>
       <c r="B143" s="8"/>
       <c r="C143" s="22" t="s">
         <v>154</v>
@@ -6788,8 +6750,8 @@
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A144" s="62"/>
+    <row r="144" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A144" s="63"/>
       <c r="B144" s="8"/>
       <c r="C144" s="24" t="s">
         <v>102</v>
@@ -6799,7 +6761,7 @@
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A145" s="62"/>
+      <c r="A145" s="63"/>
       <c r="B145" s="8"/>
       <c r="C145" s="41" t="s">
         <v>114</v>
@@ -6809,7 +6771,7 @@
       </c>
     </row>
     <row r="146" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A146" s="62"/>
+      <c r="A146" s="63"/>
       <c r="B146" s="8"/>
       <c r="C146" s="31" t="s">
         <v>41</v>
@@ -6819,27 +6781,27 @@
       </c>
     </row>
     <row r="147" spans="1:7" ht="290" x14ac:dyDescent="0.35">
-      <c r="A147" s="62"/>
+      <c r="A147" s="63"/>
       <c r="B147" s="8"/>
       <c r="C147" s="21" t="s">
         <v>178</v>
       </c>
       <c r="D147" s="21" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="148" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A148" s="62"/>
+      <c r="A148" s="63"/>
       <c r="B148" s="8"/>
       <c r="C148" s="29" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D148" s="29" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="149" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A149" s="62"/>
+      <c r="A149" s="63"/>
       <c r="B149" s="8"/>
       <c r="C149" s="22" t="s">
         <v>105</v>
@@ -6849,7 +6811,7 @@
       </c>
     </row>
     <row r="150" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A150" s="62"/>
+      <c r="A150" s="63"/>
       <c r="B150" s="8"/>
       <c r="C150" s="24" t="s">
         <v>102</v>
@@ -6859,49 +6821,49 @@
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A151" s="62"/>
+      <c r="A151" s="63"/>
       <c r="B151" s="8"/>
       <c r="C151" s="41" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A152" s="62"/>
+      <c r="A152" s="63"/>
       <c r="B152" s="8"/>
       <c r="C152" s="31" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="153" spans="1:7" ht="275.5" x14ac:dyDescent="0.35">
-      <c r="A153" s="62"/>
+      <c r="A153" s="63"/>
       <c r="B153" s="8"/>
       <c r="C153" s="21" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="154" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A154" s="62"/>
+      <c r="A154" s="63"/>
       <c r="B154" s="8"/>
       <c r="C154" s="29" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="155" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A155" s="62"/>
+      <c r="A155" s="63"/>
       <c r="B155" s="8"/>
       <c r="C155" s="22" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="156" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A156" s="62"/>
+      <c r="A156" s="63"/>
       <c r="B156" s="8"/>
       <c r="C156" s="24" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="157" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A157" s="63" t="s">
+      <c r="A157" s="64" t="s">
         <v>76</v>
       </c>
       <c r="B157" s="7" t="s">
@@ -6924,7 +6886,7 @@
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A158" s="63"/>
+      <c r="A158" s="64"/>
       <c r="B158" s="8"/>
       <c r="C158" s="31" t="s">
         <v>90</v>
@@ -6940,7 +6902,7 @@
       </c>
     </row>
     <row r="159" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A159" s="63"/>
+      <c r="A159" s="64"/>
       <c r="B159" s="8" t="s">
         <v>41</v>
       </c>
@@ -6958,7 +6920,7 @@
       </c>
     </row>
     <row r="160" spans="1:7" ht="332.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A160" s="63"/>
+      <c r="A160" s="64"/>
       <c r="B160" s="8" t="s">
         <v>180</v>
       </c>
@@ -6976,17 +6938,17 @@
       </c>
     </row>
     <row r="161" spans="1:7" ht="145" x14ac:dyDescent="0.35">
-      <c r="A161" s="63"/>
+      <c r="A161" s="64"/>
       <c r="B161" s="8" t="s">
         <v>181</v>
       </c>
       <c r="C161" s="29"/>
       <c r="E161" s="29" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="162" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A162" s="63"/>
+      <c r="A162" s="64"/>
       <c r="B162" s="15" t="s">
         <v>47</v>
       </c>
@@ -6996,7 +6958,7 @@
       </c>
     </row>
     <row r="163" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A163" s="63"/>
+      <c r="A163" s="64"/>
       <c r="B163" s="13" t="s">
         <v>52</v>
       </c>
@@ -7006,7 +6968,7 @@
       </c>
     </row>
     <row r="164" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A164" s="63" t="s">
+      <c r="A164" s="64" t="s">
         <v>78</v>
       </c>
       <c r="B164" s="7" t="s">
@@ -7029,7 +6991,7 @@
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A165" s="63"/>
+      <c r="A165" s="64"/>
       <c r="B165" s="8"/>
       <c r="C165" s="46"/>
       <c r="D165" s="41" t="s">
@@ -7039,7 +7001,7 @@
       <c r="F165" s="46"/>
     </row>
     <row r="166" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A166" s="63"/>
+      <c r="A166" s="64"/>
       <c r="B166" s="8" t="s">
         <v>41</v>
       </c>
@@ -7057,7 +7019,7 @@
       </c>
     </row>
     <row r="167" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A167" s="63"/>
+      <c r="A167" s="64"/>
       <c r="B167" s="8" t="s">
         <v>180</v>
       </c>
@@ -7075,17 +7037,17 @@
       </c>
     </row>
     <row r="168" spans="1:7" ht="145" x14ac:dyDescent="0.35">
-      <c r="A168" s="63"/>
+      <c r="A168" s="64"/>
       <c r="B168" s="8" t="s">
         <v>182</v>
       </c>
       <c r="C168" s="29"/>
       <c r="D168" s="29" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="169" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A169" s="63"/>
+      <c r="A169" s="64"/>
       <c r="B169" s="15" t="s">
         <v>47</v>
       </c>
@@ -7095,7 +7057,7 @@
       </c>
     </row>
     <row r="170" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A170" s="63"/>
+      <c r="A170" s="64"/>
       <c r="B170" s="13" t="s">
         <v>52</v>
       </c>
@@ -7105,7 +7067,7 @@
       </c>
     </row>
     <row r="171" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A171" s="63" t="s">
+      <c r="A171" s="64" t="s">
         <v>80</v>
       </c>
       <c r="B171" s="7" t="s">
@@ -7128,7 +7090,7 @@
       </c>
     </row>
     <row r="172" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A172" s="63"/>
+      <c r="A172" s="64"/>
       <c r="B172" s="8" t="s">
         <v>41</v>
       </c>
@@ -7146,7 +7108,7 @@
       </c>
     </row>
     <row r="173" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A173" s="63"/>
+      <c r="A173" s="64"/>
       <c r="B173" s="8" t="s">
         <v>180</v>
       </c>
@@ -7164,14 +7126,14 @@
       </c>
     </row>
     <row r="174" spans="1:7" ht="145" x14ac:dyDescent="0.35">
-      <c r="A174" s="63"/>
+      <c r="A174" s="64"/>
       <c r="B174" s="8" t="s">
         <v>183</v>
       </c>
       <c r="C174" s="29"/>
     </row>
     <row r="175" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A175" s="63"/>
+      <c r="A175" s="64"/>
       <c r="B175" s="15" t="s">
         <v>47</v>
       </c>
@@ -7185,7 +7147,7 @@
       <c r="C176" s="29"/>
     </row>
     <row r="177" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A177" s="63" t="s">
+      <c r="A177" s="64" t="s">
         <v>82</v>
       </c>
       <c r="B177" s="7" t="s">
@@ -7208,7 +7170,7 @@
       </c>
     </row>
     <row r="178" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A178" s="63"/>
+      <c r="A178" s="64"/>
       <c r="B178" s="8" t="s">
         <v>41</v>
       </c>
@@ -7226,7 +7188,7 @@
       </c>
     </row>
     <row r="179" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A179" s="63"/>
+      <c r="A179" s="64"/>
       <c r="B179" s="8" t="s">
         <v>180</v>
       </c>
@@ -7244,13 +7206,13 @@
       </c>
     </row>
     <row r="180" spans="1:7" ht="145" x14ac:dyDescent="0.35">
-      <c r="A180" s="63"/>
+      <c r="A180" s="64"/>
       <c r="B180" s="8" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="181" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A181" s="63"/>
+      <c r="A181" s="64"/>
       <c r="B181" s="8" t="s">
         <v>47</v>
       </c>
@@ -7259,7 +7221,7 @@
       </c>
     </row>
     <row r="182" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A182" s="63"/>
+      <c r="A182" s="64"/>
       <c r="B182" s="16" t="s">
         <v>52</v>
       </c>
@@ -7268,7 +7230,7 @@
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A183" s="63"/>
+      <c r="A183" s="64"/>
       <c r="C183" s="29"/>
     </row>
     <row r="184" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
@@ -7394,6 +7356,16 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="A177:A183"/>
     <mergeCell ref="A59:A62"/>
@@ -7409,16 +7381,6 @@
     <mergeCell ref="A164:A170"/>
     <mergeCell ref="A50:A53"/>
     <mergeCell ref="A54:A58"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
Added documentation of each testcases. Fixes #141
</commit_message>
<xml_diff>
--- a/testing/OamLog+testcase.docs.xlsx
+++ b/testing/OamLog+testcase.docs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venka\Documents\MW\OL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venka\MW_Testing\OamLog_Documentation\OamLog\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5137041-03DF-4F47-A6D6-85FC39E47E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF29CC5E-55A1-442A-B45E-712F728D6A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{8A4BF7CC-909B-4C1B-B59F-29AF2D960B3A}"/>
   </bookViews>
@@ -511,9 +511,6 @@
     <t>## Get release-number checked for correctness?</t>
   </si>
   <si>
-    <t>AdministratorAdministration</t>
-  </si>
-  <si>
     <t>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
@@ -1381,6 +1378,9 @@
    - checking response 
    - checking same record for containing DummyXCorrelator and applicatin-name and release-number with randomly chosen values.
 </t>
+  </si>
+  <si>
+    <t>OamLog</t>
   </si>
 </sst>
 </file>
@@ -2178,10 +2178,10 @@
   <dimension ref="A1:I223"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B117" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B110" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D119" sqref="D119"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2198,7 +2198,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A1" s="54" t="s">
-        <v>122</v>
+        <v>225</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="17"/>
@@ -2241,13 +2241,13 @@
         <v>88</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H3" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="I3" s="19" t="s">
         <v>216</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -2292,7 +2292,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D5" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -2450,7 +2450,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D7" s="23" t="str">
         <f>$B7</f>
@@ -2525,7 +2525,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D9" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -2680,7 +2680,7 @@
 - not applicable</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D11" s="26" t="str">
         <f>$B7</f>
@@ -2755,7 +2755,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D13" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -2911,7 +2911,7 @@
 - not applicable</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D15" s="23" t="str">
         <f>$B7</f>
@@ -2986,7 +2986,7 @@
         <v>18</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D17" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -3141,7 +3141,7 @@
 - not applicable</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D19" s="30" t="str">
         <f>$B7</f>
@@ -3216,7 +3216,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D21" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -3371,7 +3371,7 @@
 - not applicable</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D23" s="30" t="str">
         <f>$B7</f>
@@ -3446,7 +3446,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D25" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -3580,7 +3580,7 @@
 - not applicable</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D27" s="23" t="str">
         <f>$B7</f>
@@ -3655,7 +3655,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D29" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -3789,7 +3789,7 @@
 - not applicable</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D31" s="23" t="str">
         <f>$B7</f>
@@ -3977,7 +3977,7 @@
 - not applicable</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D35" s="30" t="str">
         <f>$B7</f>
@@ -4168,7 +4168,7 @@
 - not applicable</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D39" s="23" t="str">
         <f>$B7</f>
@@ -4385,7 +4385,7 @@
 - not applicable</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D43" s="23" t="str">
         <f>$B7</f>
@@ -4477,10 +4477,10 @@
     <row r="46" spans="1:9" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A46" s="64"/>
       <c r="B46" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D46" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -4646,7 +4646,7 @@
     <row r="47" spans="1:9" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A47" s="64"/>
       <c r="B47" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C47" s="29" t="str">
         <f t="shared" ref="C47:I47" si="29">CONCATENATE("#### Testing:
@@ -4733,7 +4733,7 @@
 - not applicable</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D48" s="32" t="str">
         <f t="shared" ref="D48:I48" si="30">$B7</f>
@@ -4799,7 +4799,7 @@
         <v>44</v>
       </c>
       <c r="G50" s="34" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H50" s="34" t="s">
         <v>44</v>
@@ -4887,7 +4887,7 @@
         <v>90</v>
       </c>
       <c r="F52" s="51" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G52" s="51"/>
       <c r="H52" s="24" t="s">
@@ -5048,7 +5048,7 @@
         <v>90</v>
       </c>
       <c r="F58" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G58" s="52" t="s">
         <v>90</v>
@@ -5096,7 +5096,7 @@
         <v>55</v>
       </c>
       <c r="C60" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D60" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -5246,7 +5246,7 @@
         <v>57</v>
       </c>
       <c r="C62" s="38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D62" s="38" t="s">
         <v>57</v>
@@ -5301,7 +5301,7 @@
         <v>60</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D64" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -5420,7 +5420,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="63" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>62</v>
@@ -5469,7 +5469,7 @@
       <c r="A69" s="63"/>
       <c r="B69" s="8"/>
       <c r="C69" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D69" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -5566,7 +5566,7 @@
       <c r="A72" s="63"/>
       <c r="B72" s="8"/>
       <c r="C72" s="41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D72" s="41" t="s">
         <v>121</v>
@@ -5579,7 +5579,7 @@
       <c r="A73" s="63"/>
       <c r="B73" s="8"/>
       <c r="C73" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D73" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -5663,17 +5663,17 @@
         <v>95</v>
       </c>
       <c r="D76" s="41" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G76" s="41" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="203" x14ac:dyDescent="0.35">
       <c r="A77" s="63"/>
       <c r="B77" s="8"/>
       <c r="C77" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D77" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -5757,17 +5757,17 @@
         <v>96</v>
       </c>
       <c r="D80" s="41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G80" s="41" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="203" x14ac:dyDescent="0.35">
       <c r="A81" s="63"/>
       <c r="B81" s="8"/>
       <c r="C81" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D81" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -5849,7 +5849,7 @@
       <c r="B84" s="8"/>
       <c r="C84" s="22"/>
       <c r="D84" s="41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
@@ -5930,7 +5930,7 @@
       <c r="A89" s="63"/>
       <c r="B89" s="8"/>
       <c r="C89" s="41" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D89" s="41" t="s">
         <v>98</v>
@@ -5942,7 +5942,7 @@
         <v>90</v>
       </c>
       <c r="G89" s="41" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="303" customHeight="1" x14ac:dyDescent="0.35">
@@ -5951,19 +5951,19 @@
         <v>65</v>
       </c>
       <c r="C90" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D90" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E90" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F90" s="52" t="s">
         <v>90</v>
       </c>
       <c r="G90" s="21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="105.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5972,19 +5972,19 @@
         <v>66</v>
       </c>
       <c r="C91" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="D91" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="E91" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="D91" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="E91" s="25" t="s">
-        <v>172</v>
-      </c>
       <c r="F91" s="52" t="s">
         <v>90</v>
       </c>
       <c r="G91" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
@@ -5993,7 +5993,7 @@
         <v>47</v>
       </c>
       <c r="C92" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D92" s="22" t="s">
         <v>100</v>
@@ -6023,7 +6023,7 @@
         <v>102</v>
       </c>
       <c r="G93" s="24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
@@ -6033,7 +6033,7 @@
         <v>97</v>
       </c>
       <c r="D94" s="41" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E94" s="41" t="s">
         <v>90</v>
@@ -6049,10 +6049,10 @@
         <v>65</v>
       </c>
       <c r="C95" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D95" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E95" s="21"/>
       <c r="F95" s="52" t="s">
@@ -6068,10 +6068,10 @@
         <v>66</v>
       </c>
       <c r="C96" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D96" s="25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E96" s="25"/>
       <c r="F96" s="52" t="s">
@@ -6085,10 +6085,10 @@
         <v>47</v>
       </c>
       <c r="C97" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D97" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E97" s="22"/>
       <c r="F97" s="52" t="s">
@@ -6114,40 +6114,40 @@
       <c r="A99" s="55"/>
       <c r="B99" s="8"/>
       <c r="C99" s="41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D99" s="41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A100" s="55"/>
       <c r="B100" s="8"/>
       <c r="C100" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D100" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A101" s="55"/>
       <c r="B101" s="8"/>
       <c r="C101" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D101" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A102" s="55"/>
       <c r="B102" s="8"/>
       <c r="C102" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D102" s="25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -6167,17 +6167,17 @@
         <v>103</v>
       </c>
       <c r="D104" s="41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="203" x14ac:dyDescent="0.35">
       <c r="A105" s="55"/>
       <c r="B105" s="8"/>
       <c r="C105" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D105" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
@@ -6187,7 +6187,7 @@
         <v>104</v>
       </c>
       <c r="D106" s="25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -6197,7 +6197,7 @@
         <v>105</v>
       </c>
       <c r="D107" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -6221,7 +6221,7 @@
       <c r="A110" s="55"/>
       <c r="B110" s="8"/>
       <c r="C110" s="21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
@@ -6313,13 +6313,13 @@
     <row r="117" spans="1:7" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A117" s="64"/>
       <c r="B117" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C117" s="44" t="s">
         <v>193</v>
       </c>
-      <c r="C117" s="44" t="s">
-        <v>194</v>
-      </c>
       <c r="D117" s="44" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E117" s="43" t="s">
         <v>90</v>
@@ -6334,13 +6334,13 @@
     <row r="118" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A118" s="64"/>
       <c r="B118" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C118" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D118" s="31" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E118" s="43" t="s">
         <v>90</v>
@@ -6393,7 +6393,7 @@
         <v>71</v>
       </c>
       <c r="E120" s="34" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F120" s="34" t="s">
         <v>71</v>
@@ -6409,7 +6409,7 @@
         <v>90</v>
       </c>
       <c r="D121" s="39" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E121" s="39" t="s">
         <v>110</v>
@@ -6430,10 +6430,10 @@
         <v>90</v>
       </c>
       <c r="D122" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E122" s="21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F122" s="39" t="s">
         <v>90</v>
@@ -6451,10 +6451,10 @@
         <v>90</v>
       </c>
       <c r="D123" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E123" s="24" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F123" s="39" t="s">
         <v>90</v>
@@ -6516,7 +6516,7 @@
       <c r="A127" s="63"/>
       <c r="B127" s="8"/>
       <c r="C127" s="41" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D127" s="41" t="s">
         <v>113</v>
@@ -6555,13 +6555,13 @@
     <row r="129" spans="1:7" ht="388.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="63"/>
       <c r="B129" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C129" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="C129" s="21" t="s">
-        <v>189</v>
-      </c>
       <c r="D129" s="21" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E129" s="39" t="s">
         <v>90</v>
@@ -6576,13 +6576,13 @@
     <row r="130" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A130" s="63"/>
       <c r="B130" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C130" s="29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D130" s="29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
@@ -6591,7 +6591,7 @@
         <v>47</v>
       </c>
       <c r="C131" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D131" s="22" t="s">
         <v>100</v>
@@ -6616,7 +6616,7 @@
         <v>112</v>
       </c>
       <c r="D133" s="41" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E133" s="39" t="s">
         <v>90</v>
@@ -6646,13 +6646,13 @@
     <row r="135" spans="1:7" ht="290" x14ac:dyDescent="0.35">
       <c r="A135" s="63"/>
       <c r="B135" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C135" s="21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D135" s="21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E135" s="39" t="s">
         <v>90</v>
@@ -6664,13 +6664,13 @@
     <row r="136" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A136" s="63"/>
       <c r="B136" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C136" s="29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D136" s="29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="137" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
@@ -6679,10 +6679,10 @@
         <v>47</v>
       </c>
       <c r="C137" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D137" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -6701,10 +6701,10 @@
       <c r="A139" s="63"/>
       <c r="B139" s="8"/>
       <c r="C139" s="41" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D139" s="41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E139" s="52" t="s">
         <v>90</v>
@@ -6724,30 +6724,30 @@
       <c r="A141" s="63"/>
       <c r="B141" s="8"/>
       <c r="C141" s="21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D141" s="21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A142" s="63"/>
       <c r="B142" s="8"/>
       <c r="C142" s="29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D142" s="29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A143" s="63"/>
       <c r="B143" s="8"/>
       <c r="C143" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D143" s="25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="144" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -6767,7 +6767,7 @@
         <v>114</v>
       </c>
       <c r="D145" s="41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="146" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -6784,20 +6784,20 @@
       <c r="A147" s="63"/>
       <c r="B147" s="8"/>
       <c r="C147" s="21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D147" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="148" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A148" s="63"/>
       <c r="B148" s="8"/>
       <c r="C148" s="29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D148" s="29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="149" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -6807,7 +6807,7 @@
         <v>105</v>
       </c>
       <c r="D149" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -6838,14 +6838,14 @@
       <c r="A153" s="63"/>
       <c r="B153" s="8"/>
       <c r="C153" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="154" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A154" s="63"/>
       <c r="B154" s="8"/>
       <c r="C154" s="29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="155" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -6922,7 +6922,7 @@
     <row r="160" spans="1:7" ht="332.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" s="64"/>
       <c r="B160" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C160" s="31" t="s">
         <v>90</v>
@@ -6931,7 +6931,7 @@
         <v>90</v>
       </c>
       <c r="E160" s="21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F160" s="31" t="s">
         <v>90</v>
@@ -6940,11 +6940,11 @@
     <row r="161" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A161" s="64"/>
       <c r="B161" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C161" s="29"/>
       <c r="E161" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="162" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -7021,13 +7021,13 @@
     <row r="167" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A167" s="64"/>
       <c r="B167" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C167" s="29" t="s">
         <v>90</v>
       </c>
       <c r="D167" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E167" s="29" t="s">
         <v>90</v>
@@ -7039,11 +7039,11 @@
     <row r="168" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A168" s="64"/>
       <c r="B168" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C168" s="29"/>
       <c r="D168" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="169" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -7110,7 +7110,7 @@
     <row r="173" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A173" s="64"/>
       <c r="B173" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C173" s="29" t="s">
         <v>90</v>
@@ -7128,7 +7128,7 @@
     <row r="174" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A174" s="64"/>
       <c r="B174" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C174" s="29"/>
     </row>
@@ -7190,7 +7190,7 @@
     <row r="179" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A179" s="64"/>
       <c r="B179" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C179" s="52" t="s">
         <v>90</v>
@@ -7208,7 +7208,7 @@
     <row r="180" spans="1:7" ht="145" x14ac:dyDescent="0.35">
       <c r="A180" s="64"/>
       <c r="B180" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="181" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -7356,16 +7356,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="A177:A183"/>
     <mergeCell ref="A59:A62"/>
@@ -7381,6 +7371,16 @@
     <mergeCell ref="A164:A170"/>
     <mergeCell ref="A50:A53"/>
     <mergeCell ref="A54:A58"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
updated OL test case collection for comments. Updated documentation for  /v1/record-oam-request :: Acceptance :: oam record created? /v1/list-records-of-application :: Acceptance :: Response body completeness
</commit_message>
<xml_diff>
--- a/testing/OamLog+testcase.docs.xlsx
+++ b/testing/OamLog+testcase.docs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venka\MW_Testing\OamLog_Documentation\OamLog\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF29CC5E-55A1-442A-B45E-712F728D6A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2204AC-B08B-40AA-84C6-E3A845B28137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{8A4BF7CC-909B-4C1B-B59F-29AF2D960B3A}"/>
   </bookViews>
@@ -1354,22 +1354,6 @@
 NA</t>
   </si>
   <si>
-    <t>#### Preparation:
-- GETing CC (/core-model-1-4:control-construct)
-- searching CC for op-s of /v1/record-oam-request, storing operation-key
-- searching CC for op-s of /v1/list-records-of-application, storing operation-key
-- POST/v1/record-oam-request with
-  - dummy values generated for  attributes
-   -operation-key from above
-   - reasonable parameter</t>
-  </si>
-  <si>
-    <t>#### Testing:
-- checking for ResponseCode==204
-- POST /v1/list-records-of-application and store response
-- verify that received response is equal to expected attribute values ( ex: application-name = ExpectedApplicationName, release-number = expectedReleaseNumber, method= expectedMethod, resource = expectedResource, etc.)</t>
-  </si>
-  <si>
     <t xml:space="preserve">#### Testing:
 - POST ExecutionAndTraceLog/v1/list-records-of-flow with 
    - IP, protocol and port from above
@@ -1381,6 +1365,24 @@
   </si>
   <si>
     <t>OamLog</t>
+  </si>
+  <si>
+    <t>#### Preparation:
+- GETing CC (/core-model-1-4:control-construct)
+  - searching CC for op-s of /v1/record-oam-request, storing operation-key
+  - searching CC for op-s of /v1/list-records-of-application, storing operation-key
+- POST/v1/record-oam-request with
+  - dummy values generated for  attributes
+  - operation-key from above
+  - reasonable parameter</t>
+  </si>
+  <si>
+    <t>#### Testing:
+- checking for ResponseCode==204 for /v1/record-oam-request
+- POST /v1/list-records-of-application and store response
+  - verify that received response parameters is equal to expected attribute values 
+ex: application-name = ExpectedApplicationName, release-number = expectedReleaseNumber, method= expectedMethod, 
+resource = expectedResource, similarly other parameters.</t>
   </si>
 </sst>
 </file>
@@ -2178,10 +2180,10 @@
   <dimension ref="A1:I223"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B110" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="E90" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2198,7 +2200,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A1" s="54" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="17"/>
@@ -5963,7 +5965,7 @@
         <v>90</v>
       </c>
       <c r="G90" s="21" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="105.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5984,7 +5986,7 @@
         <v>90</v>
       </c>
       <c r="G91" s="25" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
@@ -6340,7 +6342,7 @@
         <v>203</v>
       </c>
       <c r="D118" s="31" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E118" s="43" t="s">
         <v>90</v>
@@ -7356,6 +7358,16 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="A177:A183"/>
     <mergeCell ref="A59:A62"/>
@@ -7371,16 +7383,6 @@
     <mergeCell ref="A164:A170"/>
     <mergeCell ref="A50:A53"/>
     <mergeCell ref="A54:A58"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
findings in test-suite Fixes #218
</commit_message>
<xml_diff>
--- a/testing/OamLog+testcase.docs.xlsx
+++ b/testing/OamLog+testcase.docs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venka\MW_Testing\OamLog_Documentation\OamLog\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IS00759329\Desktop\Telefonica\ApplicationPattern\ApplicationPattern_v2\OamLog\OamLog-2\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2204AC-B08B-40AA-84C6-E3A845B28137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4265180F-A8B9-4BDC-95D0-6F6B53FA9DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{8A4BF7CC-909B-4C1B-B59F-29AF2D960B3A}"/>
+    <workbookView xWindow="285" yWindow="270" windowWidth="20205" windowHeight="10650" xr2:uid="{8A4BF7CC-909B-4C1B-B59F-29AF2D960B3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Servicelayer" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="227">
   <si>
     <t>Testcases</t>
   </si>
@@ -1383,6 +1383,14 @@
   - verify that received response parameters is equal to expected attribute values 
 ex: application-name = ExpectedApplicationName, release-number = expectedReleaseNumber, method= expectedMethod, 
 resource = expectedResource, similarly other parameters.</t>
+  </si>
+  <si>
+    <t>#### Clearing:
+- PUT initial newRelease/application-name
+- PUT initial newRelease/release-number
+- PUT initial newRelease/protocol
+- PUT initial newRelease/address
+- PUT initial newRelease/port</t>
   </si>
 </sst>
 </file>
@@ -2179,26 +2187,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6438CD8-A3F3-4ED1-9D84-D5D573F05C15}">
   <dimension ref="A1:I223"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="E90" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B117" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G91" sqref="G91"/>
+      <selection pane="bottomRight" activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.54296875" style="58" customWidth="1"/>
-    <col min="2" max="2" width="70.7265625" style="2"/>
-    <col min="3" max="6" width="70.7265625" style="52"/>
-    <col min="7" max="7" width="70.7265625" style="52" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" style="58" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" style="2"/>
+    <col min="3" max="6" width="70.7109375" style="52"/>
+    <col min="7" max="7" width="70.7109375" style="52" customWidth="1"/>
     <col min="8" max="8" width="70" style="52" customWidth="1"/>
-    <col min="9" max="9" width="63.36328125" style="52" customWidth="1"/>
-    <col min="10" max="40" width="9.1796875" style="52" customWidth="1"/>
-    <col min="41" max="16384" width="9.1796875" style="52"/>
+    <col min="9" max="9" width="63.42578125" style="52" customWidth="1"/>
+    <col min="10" max="40" width="9.140625" style="52" customWidth="1"/>
+    <col min="41" max="16384" width="9.140625" style="52"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>223</v>
       </c>
@@ -2209,7 +2217,7 @@
       <c r="F1" s="17"/>
       <c r="G1" s="17"/>
     </row>
-    <row r="2" spans="1:9" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
         <v>0</v>
       </c>
@@ -2223,7 +2231,7 @@
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" spans="1:9" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
         <v>1</v>
       </c>
@@ -2252,7 +2260,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="63" t="s">
         <v>3</v>
       </c>
@@ -2288,7 +2296,7 @@
         <v>## Is service idempotent?</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A5" s="63"/>
       <c r="B5" s="5" t="s">
         <v>5</v>
@@ -2401,7 +2409,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="63"/>
       <c r="B6" s="5" t="s">
         <v>6</v>
@@ -2446,7 +2454,7 @@
 - checking for ResponseCode==200</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="63"/>
       <c r="B7" s="6" t="s">
         <v>7</v>
@@ -2485,7 +2493,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="63" t="s">
         <v>8</v>
       </c>
@@ -2521,7 +2529,7 @@
         <v>## Get parameters checked for completeness?</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A9" s="63"/>
       <c r="B9" s="8" t="s">
         <v>10</v>
@@ -2633,7 +2641,7 @@
     - BUT one randomly chosen parameter (user, originator, x-correlator, trace-indicator or customer-journey) missing (not empty string!)</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="63"/>
       <c r="B10" s="8" t="s">
         <v>11</v>
@@ -2674,7 +2682,7 @@
 - checking for ResponseCode == 400</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="63"/>
       <c r="B11" s="6" t="str">
         <f>$B7</f>
@@ -2715,7 +2723,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="63" t="s">
         <v>12</v>
       </c>
@@ -2751,7 +2759,7 @@
         <v>## Gets originator checked for compliance with specification?</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="203" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A13" s="63"/>
       <c r="B13" s="8" t="s">
         <v>14</v>
@@ -2864,7 +2872,7 @@
           1.  originator set to be a string of 0, 1 or 2 (random) letters length (too short).</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="63"/>
       <c r="B14" s="8" t="s">
         <v>15</v>
@@ -2905,7 +2913,7 @@
 - checking for ResponseCode==400</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="63"/>
       <c r="B15" s="6" t="str">
         <f>$B7</f>
@@ -2946,7 +2954,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="63" t="s">
         <v>16</v>
       </c>
@@ -2982,7 +2990,7 @@
         <v>## Gets x-correlator checked for complying the pattern?</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="203" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A17" s="63"/>
       <c r="B17" s="8" t="s">
         <v>18</v>
@@ -3094,7 +3102,7 @@
     - reasonable parameters, BUT dummyXCorrelators differing from the pattern in various ways (e.g. empty string)</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="63"/>
       <c r="B18" s="8" t="s">
         <v>15</v>
@@ -3135,7 +3143,7 @@
 - checking for ResponseCode==400</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="63"/>
       <c r="B19" s="6" t="str">
         <f>$B7</f>
@@ -3176,7 +3184,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="63" t="s">
         <v>19</v>
       </c>
@@ -3212,7 +3220,7 @@
         <v>## Gets trace-indicator checked for complying the pattern?</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="203" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A21" s="63"/>
       <c r="B21" s="8" t="s">
         <v>21</v>
@@ -3324,7 +3332,7 @@
     - reasonable parameters, BUT dummyTraceIndicator differing from the pattern in various ways (e.g. empty string)</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="63"/>
       <c r="B22" s="8" t="s">
         <v>15</v>
@@ -3365,7 +3373,7 @@
 - checking for ResponseCode==400</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="63"/>
       <c r="B23" s="6" t="str">
         <f>$B7</f>
@@ -3406,7 +3414,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="63" t="s">
         <v>22</v>
       </c>
@@ -3442,7 +3450,7 @@
         <v>## Gets security key checked for availability?</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A25" s="63"/>
       <c r="B25" s="8" t="s">
         <v>24</v>
@@ -3533,7 +3541,7 @@
     - BUT operationKey parameter missing (does not mean empty string)</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="63"/>
       <c r="B26" s="8" t="s">
         <v>25</v>
@@ -3574,7 +3582,7 @@
 - checking for ResponseCode==401</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="63"/>
       <c r="B27" s="6" t="str">
         <f>$B7</f>
@@ -3615,7 +3623,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="63" t="s">
         <v>26</v>
       </c>
@@ -3651,7 +3659,7 @@
         <v>## Gets security key checked for correctness?</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A29" s="63"/>
       <c r="B29" s="8" t="s">
         <v>28</v>
@@ -3742,7 +3750,7 @@
      - BUT operationKey parameter with random dummy value</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="63"/>
       <c r="B30" s="8" t="s">
         <v>25</v>
@@ -3783,7 +3791,7 @@
 - checking for ResponseCode==401</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="63"/>
       <c r="B31" s="6" t="str">
         <f>$B7</f>
@@ -3824,7 +3832,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="63" t="s">
         <v>29</v>
       </c>
@@ -3860,7 +3868,7 @@
         <v>## Contains response complete set of headers?</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A33" s="63"/>
       <c r="B33" s="8" t="s">
         <v>31</v>
@@ -3938,7 +3946,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="63"/>
       <c r="B34" s="8" t="s">
         <v>32</v>
@@ -3971,7 +3979,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="63"/>
       <c r="B35" s="6" t="str">
         <f>$B7</f>
@@ -4012,7 +4020,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="63" t="s">
         <v>33</v>
       </c>
@@ -4048,7 +4056,7 @@
         <v>## Is the initial x-correlator ín the response?</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A37" s="63"/>
       <c r="B37" s="8" t="s">
         <v>31</v>
@@ -4126,7 +4134,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="63"/>
       <c r="B38" s="8" t="s">
         <v>35</v>
@@ -4162,7 +4170,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="63"/>
       <c r="B39" s="6" t="str">
         <f>$B7</f>
@@ -4203,7 +4211,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="63" t="s">
         <v>36</v>
       </c>
@@ -4239,7 +4247,7 @@
         <v>## Is the correct life-cycle-state ín the response?</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A41" s="64"/>
       <c r="B41" s="8" t="s">
         <v>31</v>
@@ -4317,7 +4325,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="64"/>
       <c r="B42" s="8" t="s">
         <v>38</v>
@@ -4379,7 +4387,7 @@
 - checking for response headers containing life-cycle-state is equal to the value as present in the control-construct for /v1/list-records-of-application/configuration/life-cycle-state</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="64"/>
       <c r="B43" s="6" t="str">
         <f>$B7</f>
@@ -4420,7 +4428,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="63" t="s">
         <v>39</v>
       </c>
@@ -4449,7 +4457,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="64"/>
       <c r="B45" s="8" t="s">
         <v>41</v>
@@ -4476,7 +4484,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" ht="300" x14ac:dyDescent="0.25">
       <c r="A46" s="64"/>
       <c r="B46" s="8" t="s">
         <v>184</v>
@@ -4645,7 +4653,7 @@
   - reasonable parameters</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A47" s="64"/>
       <c r="B47" s="8" t="s">
         <v>185</v>
@@ -4727,7 +4735,7 @@
    - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="64"/>
       <c r="B48" s="9" t="str">
         <f>$B7</f>
@@ -4768,7 +4776,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="56" t="s">
         <v>42</v>
       </c>
@@ -4781,7 +4789,7 @@
       <c r="H49" s="3"/>
       <c r="I49" s="62"/>
     </row>
-    <row r="50" spans="1:9" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A50" s="65" t="s">
         <v>43</v>
       </c>
@@ -4810,7 +4818,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="153.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" ht="153.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="63"/>
       <c r="B51" s="12" t="s">
         <v>45</v>
@@ -4874,7 +4882,7 @@
       - reasonable parameters </v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="171" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" ht="171" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="63"/>
       <c r="B52" s="13" t="s">
         <v>46</v>
@@ -4899,7 +4907,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="63"/>
       <c r="B53" s="14" t="s">
         <v>47</v>
@@ -4930,7 +4938,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="64" t="s">
         <v>48</v>
       </c>
@@ -4953,7 +4961,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="174" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A55" s="64"/>
       <c r="B55" s="12" t="s">
         <v>50</v>
@@ -4995,7 +5003,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="64"/>
       <c r="B56" s="13" t="s">
         <v>51</v>
@@ -5016,7 +5024,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="64"/>
       <c r="B57" s="14" t="s">
         <v>47</v>
@@ -5037,7 +5045,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="64"/>
       <c r="B58" s="13" t="s">
         <v>52</v>
@@ -5056,7 +5064,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="63" t="s">
         <v>53</v>
       </c>
@@ -5092,7 +5100,7 @@
         <v>## Gets lifeCycleState propagated?</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="203" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A60" s="64"/>
       <c r="B60" s="8" t="s">
         <v>55</v>
@@ -5215,7 +5223,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="64"/>
       <c r="B61" s="8" t="s">
         <v>56</v>
@@ -5242,7 +5250,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="64"/>
       <c r="B62" s="15" t="s">
         <v>57</v>
@@ -5269,7 +5277,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="63" t="s">
         <v>58</v>
       </c>
@@ -5297,7 +5305,7 @@
         <v>## Get attributes checked for completeness?</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="203" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A64" s="63"/>
       <c r="B64" s="8" t="s">
         <v>60</v>
@@ -5362,7 +5370,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="63"/>
       <c r="B65" s="8" t="s">
         <v>61</v>
@@ -5391,7 +5399,7 @@
 - checking for ResponseCode==400</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="63"/>
       <c r="B66" s="15" t="s">
         <v>47</v>
@@ -5420,7 +5428,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="63" t="s">
         <v>132</v>
       </c>
@@ -5448,7 +5456,7 @@
         <v>## Get each attributes checked for correctness?</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="63"/>
       <c r="B68" s="8"/>
       <c r="C68" s="41" t="s">
@@ -5467,7 +5475,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="225" x14ac:dyDescent="0.25">
       <c r="A69" s="63"/>
       <c r="B69" s="8"/>
       <c r="C69" s="21" t="s">
@@ -5520,7 +5528,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="63"/>
       <c r="B70" s="8"/>
       <c r="C70" s="25" t="str">
@@ -5540,7 +5548,7 @@
 - checking for ResponseCode==400</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="63"/>
       <c r="B71" s="8"/>
       <c r="C71" s="22" t="str">
@@ -5564,7 +5572,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="63"/>
       <c r="B72" s="8"/>
       <c r="C72" s="41" t="s">
@@ -5577,7 +5585,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="A73" s="63"/>
       <c r="B73" s="8"/>
       <c r="C73" s="21" t="s">
@@ -5620,7 +5628,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="63"/>
       <c r="B74" s="8"/>
       <c r="C74" s="25" t="str">
@@ -5639,7 +5647,7 @@
 - checking for ResponseCode==400</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="63"/>
       <c r="B75" s="8"/>
       <c r="C75" s="50" t="str">
@@ -5658,7 +5666,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="63"/>
       <c r="B76" s="8"/>
       <c r="C76" s="41" t="s">
@@ -5671,7 +5679,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="A77" s="63"/>
       <c r="B77" s="8"/>
       <c r="C77" s="21" t="s">
@@ -5714,7 +5722,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="63"/>
       <c r="B78" s="8"/>
       <c r="C78" s="25" t="str">
@@ -5733,7 +5741,7 @@
 - checking for ResponseCode==400</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="63"/>
       <c r="B79" s="8"/>
       <c r="C79" s="22" t="str">
@@ -5752,7 +5760,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="63"/>
       <c r="B80" s="8"/>
       <c r="C80" s="41" t="s">
@@ -5765,7 +5773,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" ht="255" x14ac:dyDescent="0.25">
       <c r="A81" s="63"/>
       <c r="B81" s="8"/>
       <c r="C81" s="21" t="s">
@@ -5808,7 +5816,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="63"/>
       <c r="B82" s="8"/>
       <c r="C82" s="25" t="str">
@@ -5827,7 +5835,7 @@
 - checking for ResponseCode==400</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="63"/>
       <c r="B83" s="8"/>
       <c r="C83" s="22" t="str">
@@ -5846,7 +5854,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="63"/>
       <c r="B84" s="8"/>
       <c r="C84" s="22"/>
@@ -5854,7 +5862,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A85" s="63"/>
       <c r="B85" s="8"/>
       <c r="C85" s="22"/>
@@ -5878,7 +5886,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="63"/>
       <c r="B86" s="8"/>
       <c r="C86" s="22"/>
@@ -5889,7 +5897,7 @@
       </c>
       <c r="G86" s="21"/>
     </row>
-    <row r="87" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="63"/>
       <c r="B87" s="8"/>
       <c r="C87" s="22"/>
@@ -5900,7 +5908,7 @@
       </c>
       <c r="G87" s="25"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="63" t="s">
         <v>63</v>
       </c>
@@ -5928,7 +5936,7 @@
         <v>## Get each attributes checked if getting correctly updated?</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="63"/>
       <c r="B89" s="8"/>
       <c r="C89" s="41" t="s">
@@ -5947,7 +5955,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="303" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" ht="303" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="64"/>
       <c r="B90" s="8" t="s">
         <v>65</v>
@@ -5968,7 +5976,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="105.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" ht="105.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="64"/>
       <c r="B91" s="8" t="s">
         <v>66</v>
@@ -5989,7 +5997,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A92" s="64"/>
       <c r="B92" s="8" t="s">
         <v>47</v>
@@ -6010,7 +6018,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A93" s="55"/>
       <c r="B93" s="13" t="s">
         <v>52</v>
@@ -6028,7 +6036,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="63"/>
       <c r="B94" s="8"/>
       <c r="C94" s="41" t="s">
@@ -6045,7 +6053,7 @@
       </c>
       <c r="G94" s="41"/>
     </row>
-    <row r="95" spans="1:7" ht="250.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" ht="250.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="64"/>
       <c r="B95" s="8" t="s">
         <v>65</v>
@@ -6064,7 +6072,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A96" s="64"/>
       <c r="B96" s="8" t="s">
         <v>66</v>
@@ -6081,7 +6089,7 @@
       </c>
       <c r="G96" s="25"/>
     </row>
-    <row r="97" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" s="64"/>
       <c r="B97" s="8" t="s">
         <v>47</v>
@@ -6098,7 +6106,7 @@
       </c>
       <c r="G97" s="22"/>
     </row>
-    <row r="98" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A98" s="55"/>
       <c r="B98" s="13" t="s">
         <v>52</v>
@@ -6112,7 +6120,7 @@
       <c r="E98" s="24"/>
       <c r="G98" s="24"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="55"/>
       <c r="B99" s="8"/>
       <c r="C99" s="41" t="s">
@@ -6122,7 +6130,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" ht="225" x14ac:dyDescent="0.25">
       <c r="A100" s="55"/>
       <c r="B100" s="8"/>
       <c r="C100" s="21" t="s">
@@ -6132,7 +6140,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A101" s="55"/>
       <c r="B101" s="8"/>
       <c r="C101" s="25" t="s">
@@ -6142,7 +6150,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="55"/>
       <c r="B102" s="8"/>
       <c r="C102" s="22" t="s">
@@ -6152,7 +6160,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A103" s="55"/>
       <c r="B103" s="8"/>
       <c r="C103" s="24" t="s">
@@ -6162,7 +6170,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="55"/>
       <c r="B104" s="8"/>
       <c r="C104" s="41" t="s">
@@ -6172,7 +6180,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="A105" s="55"/>
       <c r="B105" s="8"/>
       <c r="C105" s="21" t="s">
@@ -6182,7 +6190,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A106" s="55"/>
       <c r="B106" s="8"/>
       <c r="C106" s="25" t="s">
@@ -6192,7 +6200,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="55"/>
       <c r="B107" s="8"/>
       <c r="C107" s="22" t="s">
@@ -6202,7 +6210,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A108" s="55"/>
       <c r="B108" s="8"/>
       <c r="C108" s="24" t="s">
@@ -6212,42 +6220,42 @@
         <v>102</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="55"/>
       <c r="B109" s="8"/>
       <c r="C109" s="41" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="A110" s="55"/>
       <c r="B110" s="8"/>
       <c r="C110" s="21" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A111" s="55"/>
       <c r="B111" s="8"/>
       <c r="C111" s="25" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="55"/>
       <c r="B112" s="8"/>
       <c r="C112" s="22" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A113" s="55"/>
       <c r="B113" s="8"/>
       <c r="C113" s="24" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="63" t="s">
         <v>67</v>
       </c>
@@ -6270,7 +6278,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="63"/>
       <c r="B115" s="12"/>
       <c r="C115" s="42" t="s">
@@ -6287,7 +6295,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="64"/>
       <c r="B116" s="8" t="s">
         <v>69</v>
@@ -6312,7 +6320,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" ht="330" x14ac:dyDescent="0.25">
       <c r="A117" s="64"/>
       <c r="B117" s="8" t="s">
         <v>192</v>
@@ -6333,7 +6341,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A118" s="64"/>
       <c r="B118" s="8" t="s">
         <v>186</v>
@@ -6354,17 +6362,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A119" s="64"/>
       <c r="B119" s="5" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
-      <c r="C119" s="45" t="str">
-        <f>$B7</f>
-        <v>#### Clearing:
-- not applicable</v>
+      <c r="C119" s="45" t="s">
+        <v>226</v>
       </c>
       <c r="D119" s="45" t="str">
         <f>$B7</f>
@@ -6381,7 +6387,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="63" t="s">
         <v>70</v>
       </c>
@@ -6404,7 +6410,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="63"/>
       <c r="B121" s="13"/>
       <c r="C121" s="39" t="s">
@@ -6423,7 +6429,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="237.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" ht="237.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="63"/>
       <c r="B122" s="12" t="s">
         <v>72</v>
@@ -6444,7 +6450,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A123" s="63"/>
       <c r="B123" s="13" t="s">
         <v>73</v>
@@ -6465,7 +6471,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A124" s="63"/>
       <c r="B124" s="13" t="s">
         <v>47</v>
@@ -6478,7 +6484,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A125" s="63"/>
       <c r="B125" s="13" t="s">
         <v>52</v>
@@ -6491,7 +6497,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="63" t="s">
         <v>74</v>
       </c>
@@ -6514,7 +6520,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="63"/>
       <c r="B127" s="8"/>
       <c r="C127" s="41" t="s">
@@ -6533,7 +6539,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="63"/>
       <c r="B128" s="8" t="s">
         <v>41</v>
@@ -6554,7 +6560,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="388.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:7" ht="388.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="63"/>
       <c r="B129" s="8" t="s">
         <v>187</v>
@@ -6575,7 +6581,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A130" s="63"/>
       <c r="B130" s="8" t="s">
         <v>189</v>
@@ -6587,7 +6593,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A131" s="63"/>
       <c r="B131" s="8" t="s">
         <v>47</v>
@@ -6599,7 +6605,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A132" s="63"/>
       <c r="B132" s="13" t="s">
         <v>52</v>
@@ -6611,7 +6617,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="63"/>
       <c r="B133" s="8"/>
       <c r="C133" s="41" t="s">
@@ -6627,7 +6633,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="63"/>
       <c r="B134" s="8" t="s">
         <v>41</v>
@@ -6645,7 +6651,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="290" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:7" ht="345" x14ac:dyDescent="0.25">
       <c r="A135" s="63"/>
       <c r="B135" s="8" t="s">
         <v>187</v>
@@ -6663,7 +6669,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A136" s="63"/>
       <c r="B136" s="8" t="s">
         <v>189</v>
@@ -6675,7 +6681,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A137" s="63"/>
       <c r="B137" s="8" t="s">
         <v>47</v>
@@ -6687,7 +6693,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A138" s="63"/>
       <c r="B138" s="13" t="s">
         <v>52</v>
@@ -6699,7 +6705,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="63"/>
       <c r="B139" s="8"/>
       <c r="C139" s="41" t="s">
@@ -6712,7 +6718,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="63"/>
       <c r="B140" s="8"/>
       <c r="C140" s="31" t="s">
@@ -6722,7 +6728,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:7" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="63"/>
       <c r="B141" s="8"/>
       <c r="C141" s="21" t="s">
@@ -6732,7 +6738,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A142" s="63"/>
       <c r="B142" s="8"/>
       <c r="C142" s="29" t="s">
@@ -6742,7 +6748,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="63"/>
       <c r="B143" s="8"/>
       <c r="C143" s="22" t="s">
@@ -6752,7 +6758,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A144" s="63"/>
       <c r="B144" s="8"/>
       <c r="C144" s="24" t="s">
@@ -6762,7 +6768,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="63"/>
       <c r="B145" s="8"/>
       <c r="C145" s="41" t="s">
@@ -6772,7 +6778,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="63"/>
       <c r="B146" s="8"/>
       <c r="C146" s="31" t="s">
@@ -6782,7 +6788,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="290" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:7" ht="360" x14ac:dyDescent="0.25">
       <c r="A147" s="63"/>
       <c r="B147" s="8"/>
       <c r="C147" s="21" t="s">
@@ -6792,7 +6798,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A148" s="63"/>
       <c r="B148" s="8"/>
       <c r="C148" s="29" t="s">
@@ -6802,7 +6808,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="63"/>
       <c r="B149" s="8"/>
       <c r="C149" s="22" t="s">
@@ -6812,7 +6818,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A150" s="63"/>
       <c r="B150" s="8"/>
       <c r="C150" s="24" t="s">
@@ -6822,49 +6828,49 @@
         <v>102</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="63"/>
       <c r="B151" s="8"/>
       <c r="C151" s="41" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="63"/>
       <c r="B152" s="8"/>
       <c r="C152" s="31" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:7" ht="360" x14ac:dyDescent="0.25">
       <c r="A153" s="63"/>
       <c r="B153" s="8"/>
       <c r="C153" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A154" s="63"/>
       <c r="B154" s="8"/>
       <c r="C154" s="29" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="63"/>
       <c r="B155" s="8"/>
       <c r="C155" s="22" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A156" s="63"/>
       <c r="B156" s="8"/>
       <c r="C156" s="24" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="64" t="s">
         <v>76</v>
       </c>
@@ -6887,7 +6893,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="64"/>
       <c r="B158" s="8"/>
       <c r="C158" s="31" t="s">
@@ -6903,7 +6909,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="64"/>
       <c r="B159" s="8" t="s">
         <v>41</v>
@@ -6921,7 +6927,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="332.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:7" ht="332.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="64"/>
       <c r="B160" s="8" t="s">
         <v>179</v>
@@ -6939,7 +6945,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A161" s="64"/>
       <c r="B161" s="8" t="s">
         <v>180</v>
@@ -6949,7 +6955,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="64"/>
       <c r="B162" s="15" t="s">
         <v>47</v>
@@ -6959,7 +6965,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A163" s="64"/>
       <c r="B163" s="13" t="s">
         <v>52</v>
@@ -6969,7 +6975,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="64" t="s">
         <v>78</v>
       </c>
@@ -6992,7 +6998,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="64"/>
       <c r="B165" s="8"/>
       <c r="C165" s="46"/>
@@ -7002,7 +7008,7 @@
       <c r="E165" s="46"/>
       <c r="F165" s="46"/>
     </row>
-    <row r="166" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="64"/>
       <c r="B166" s="8" t="s">
         <v>41</v>
@@ -7020,7 +7026,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="A167" s="64"/>
       <c r="B167" s="8" t="s">
         <v>179</v>
@@ -7038,7 +7044,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A168" s="64"/>
       <c r="B168" s="8" t="s">
         <v>181</v>
@@ -7048,7 +7054,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A169" s="64"/>
       <c r="B169" s="15" t="s">
         <v>47</v>
@@ -7058,7 +7064,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A170" s="64"/>
       <c r="B170" s="13" t="s">
         <v>52</v>
@@ -7068,7 +7074,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="64" t="s">
         <v>80</v>
       </c>
@@ -7091,7 +7097,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="64"/>
       <c r="B172" s="8" t="s">
         <v>41</v>
@@ -7109,7 +7115,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A173" s="64"/>
       <c r="B173" s="8" t="s">
         <v>179</v>
@@ -7127,28 +7133,28 @@
         <v>90</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A174" s="64"/>
       <c r="B174" s="8" t="s">
         <v>182</v>
       </c>
       <c r="C174" s="29"/>
     </row>
-    <row r="175" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A175" s="64"/>
       <c r="B175" s="15" t="s">
         <v>47</v>
       </c>
       <c r="C175" s="29"/>
     </row>
-    <row r="176" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="55"/>
       <c r="B176" s="13" t="s">
         <v>52</v>
       </c>
       <c r="C176" s="29"/>
     </row>
-    <row r="177" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="64" t="s">
         <v>82</v>
       </c>
@@ -7171,7 +7177,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A178" s="64"/>
       <c r="B178" s="8" t="s">
         <v>41</v>
@@ -7189,7 +7195,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A179" s="64"/>
       <c r="B179" s="8" t="s">
         <v>179</v>
@@ -7207,13 +7213,13 @@
         <v>90</v>
       </c>
     </row>
-    <row r="180" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A180" s="64"/>
       <c r="B180" s="8" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A181" s="64"/>
       <c r="B181" s="8" t="s">
         <v>47</v>
@@ -7222,7 +7228,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" s="64"/>
       <c r="B182" s="16" t="s">
         <v>52</v>
@@ -7231,143 +7237,133 @@
         <v>90</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="64"/>
       <c r="C183" s="29"/>
     </row>
-    <row r="184" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="57"/>
       <c r="C184" s="49"/>
     </row>
-    <row r="185" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="57"/>
     </row>
-    <row r="186" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="57"/>
     </row>
-    <row r="187" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A187" s="57"/>
     </row>
-    <row r="188" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A188" s="57"/>
     </row>
-    <row r="189" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A189" s="57"/>
     </row>
-    <row r="190" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A190" s="57"/>
     </row>
-    <row r="191" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="57"/>
     </row>
-    <row r="192" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A192" s="57"/>
     </row>
-    <row r="193" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A193" s="57"/>
     </row>
-    <row r="194" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="57"/>
     </row>
-    <row r="195" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="57"/>
     </row>
-    <row r="196" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="57"/>
     </row>
-    <row r="197" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="57"/>
     </row>
-    <row r="198" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="57"/>
     </row>
-    <row r="199" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A199" s="57"/>
     </row>
-    <row r="200" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A200" s="57"/>
     </row>
-    <row r="201" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A201" s="57"/>
     </row>
-    <row r="202" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A202" s="57"/>
     </row>
-    <row r="203" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A203" s="57"/>
     </row>
-    <row r="204" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A204" s="57"/>
     </row>
-    <row r="205" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A205" s="57"/>
     </row>
-    <row r="206" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A206" s="57"/>
     </row>
-    <row r="207" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A207" s="57"/>
     </row>
-    <row r="208" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A208" s="57"/>
     </row>
-    <row r="209" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A209" s="57"/>
     </row>
-    <row r="210" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A210" s="57"/>
     </row>
-    <row r="211" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A211" s="57"/>
     </row>
-    <row r="212" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A212" s="57"/>
     </row>
-    <row r="213" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A213" s="57"/>
     </row>
-    <row r="214" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A214" s="57"/>
     </row>
-    <row r="215" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A215" s="57"/>
     </row>
-    <row r="216" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A216" s="57"/>
     </row>
-    <row r="217" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A217" s="57"/>
     </row>
-    <row r="218" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A218" s="57"/>
     </row>
-    <row r="219" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" s="57"/>
     </row>
-    <row r="220" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A220" s="57"/>
     </row>
-    <row r="221" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A221" s="57"/>
     </row>
-    <row r="222" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A222" s="57"/>
     </row>
-    <row r="223" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A223" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="A177:A183"/>
     <mergeCell ref="A59:A62"/>
@@ -7383,6 +7379,16 @@
     <mergeCell ref="A164:A170"/>
     <mergeCell ref="A50:A53"/>
     <mergeCell ref="A54:A58"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>